<commit_message>
Adding the assertion to test cases and adding Register API Request
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Pixelogic.xlsx
+++ b/src/test/resources/TestDataFiles/Pixelogic.xlsx
@@ -45,16 +45,16 @@
     <t>Confirm Password</t>
   </si>
   <si>
-    <t>Ma</t>
+    <t>Magdy@123</t>
   </si>
   <si>
-    <t>He</t>
+    <t>ma5@mai.com</t>
   </si>
   <si>
-    <t>ma@mai.com</t>
+    <t>Hei</t>
   </si>
   <si>
-    <t>Magdy@123</t>
+    <t>Mag</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding some comments to the script and update Readme.md
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Pixelogic.xlsx
+++ b/src/test/resources/TestDataFiles/Pixelogic.xlsx
@@ -48,13 +48,13 @@
     <t>Magdy@123</t>
   </si>
   <si>
-    <t>ma5@mai.com</t>
-  </si>
-  <si>
     <t>Hei</t>
   </si>
   <si>
     <t>Mag</t>
+  </si>
+  <si>
+    <t>ma6@mai.com</t>
   </si>
 </sst>
 </file>
@@ -2509,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">

</xml_diff>